<commit_message>
Crear cuenta bancaria terminada
</commit_message>
<xml_diff>
--- a/MercuryTours/Resources/datapool/datosBancos.xlsx
+++ b/MercuryTours/Resources/datapool/datosBancos.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12900" windowHeight="4845"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="14520" windowHeight="5070"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Correcto</t>
   </si>
@@ -63,6 +63,51 @@
   </si>
   <si>
     <t>BANCO BBVA</t>
+  </si>
+  <si>
+    <t>codigo</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>02</t>
+  </si>
+  <si>
+    <t>03</t>
+  </si>
+  <si>
+    <t>04</t>
+  </si>
+  <si>
+    <t>05</t>
+  </si>
+  <si>
+    <t>06</t>
+  </si>
+  <si>
+    <t>07</t>
+  </si>
+  <si>
+    <t>08</t>
+  </si>
+  <si>
+    <t>09</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
   </si>
 </sst>
 </file>
@@ -98,8 +143,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -404,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -415,14 +461,15 @@
     <col min="1" max="1" width="12.5703125" customWidth="1"/>
     <col min="2" max="2" width="15.140625" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -463,14 +510,64 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="P3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B4">
         <v>123</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
muchos cambios sin importancia
</commit_message>
<xml_diff>
--- a/MercuryTours/Resources/datapool/datosBancos.xlsx
+++ b/MercuryTours/Resources/datapool/datosBancos.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14520" windowHeight="5070"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14055" windowHeight="4560"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Correcto</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>14</t>
+  </si>
+  <si>
+    <t>Bancoca</t>
   </si>
 </sst>
 </file>
@@ -453,7 +456,7 @@
   <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,6 +491,9 @@
       <c r="F2" t="s">
         <v>7</v>
       </c>
+      <c r="G2" t="s">
+        <v>31</v>
+      </c>
       <c r="H2" t="s">
         <v>8</v>
       </c>

</xml_diff>